<commit_message>
continued work on line graphs
</commit_message>
<xml_diff>
--- a/Original Plot Work/1906 - 1913 Tuberculosis Mortality Country&Town/Tuberculosis Countries.xlsx
+++ b/Original Plot Work/1906 - 1913 Tuberculosis Mortality Country&Town/Tuberculosis Countries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RBY11\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DF2A9A-B0F9-4FD4-AA8E-0EC567BAA127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B976F91-8970-4605-8B00-50DFC854D662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1410" yWindow="2400" windowWidth="21600" windowHeight="11835" xr2:uid="{DA6CF01D-ED2C-4DA0-8F2F-D3B75DC7518E}"/>
   </bookViews>
@@ -49,10 +49,10 @@
     <t>France</t>
   </si>
   <si>
-    <t>United_States</t>
+    <t>United States</t>
   </si>
   <si>
-    <t>England&amp;Wales</t>
+    <t>England &amp; Wales</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C25"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>